<commit_message>
Addition of control flow/error handling.
</commit_message>
<xml_diff>
--- a/.data/City Weather.xlsx
+++ b/.data/City Weather.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ortig-my.sharepoint.com/personal/kbunger_oldrepublictitle_com/Documents/Documents/UiPath/OpenWeather_API_Practice/.data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{507D011E-ABE9-4D85-97B9-E7262F30AC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6948613-9358-4DB4-9FE5-79F38EB8A3D3}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="8_{507D011E-ABE9-4D85-97B9-E7262F30AC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{614E8B69-D234-465D-A77D-4842A868F019}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{50C85241-72C1-4676-BDC0-1A007D98EFE2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>City Name</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Miami</t>
+  </si>
+  <si>
+    <t>Tampa Bay</t>
+  </si>
+  <si>
+    <t>Midland</t>
+  </si>
+  <si>
+    <t>Not Found</t>
   </si>
 </sst>
 </file>
@@ -149,8 +158,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82245872-9D41-4481-B1D0-80AD6268392E}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10" xr:uid="{82245872-9D41-4481-B1D0-80AD6268392E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82245872-9D41-4481-B1D0-80AD6268392E}" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12" xr:uid="{82245872-9D41-4481-B1D0-80AD6268392E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D726A1A7-7776-4BC4-9DDE-0EC75BCDBE53}" name="City Name"/>
     <tableColumn id="2" xr3:uid="{3CB72A82-65B9-495C-8429-5D4045E0C17C}" name="Temperature" dataDxfId="2"/>
@@ -458,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73016D44-1163-4C80-BD1C-1226782DAC43}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F3:F4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,45 +499,154 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="2">
+        <v>46.65</v>
+      </c>
+      <c r="C2" s="2">
+        <v>39.79</v>
+      </c>
+      <c r="D2" s="1">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="2">
+        <v>58.73</v>
+      </c>
+      <c r="C3" s="2">
+        <v>58.73</v>
+      </c>
+      <c r="D3" s="1">
+        <v>94</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="2">
+        <v>51.71</v>
+      </c>
+      <c r="C4" s="2">
+        <v>49.96</v>
+      </c>
+      <c r="D4" s="1">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="B5" s="2">
+        <v>10.87</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-1.73</v>
+      </c>
+      <c r="D5" s="1">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
+      <c r="B6" s="2">
+        <v>66.22</v>
+      </c>
+      <c r="C6" s="2">
+        <v>66.11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>76</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="B7" s="2">
+        <v>54.72</v>
+      </c>
+      <c r="C7" s="2">
+        <v>54.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="B8" s="2">
+        <v>50.29</v>
+      </c>
+      <c r="C8" s="2">
+        <v>49.15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="B9" s="2">
+        <v>35.44</v>
+      </c>
+      <c r="C9" s="2">
+        <v>28.99</v>
+      </c>
+      <c r="D9" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>51.48</v>
+      </c>
+      <c r="C10" s="2">
+        <v>49.28</v>
+      </c>
+      <c r="D10" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45.73</v>
+      </c>
+      <c r="C12" s="2">
+        <v>40.229999999999997</v>
+      </c>
+      <c r="D12" s="1">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>